<commit_message>
added blat for banca in dressing.py
</commit_message>
<xml_diff>
--- a/pythonProject/projects/Comanda Test/Comanda_Proficut_Test.xlsx
+++ b/pythonProject/projects/Comanda Test/Comanda_Proficut_Test.xlsx
@@ -2605,15 +2605,45 @@
       </c>
     </row>
     <row r="19" ht="18.75" customHeight="1" s="50">
-      <c r="A19" s="108" t="n"/>
-      <c r="B19" s="108" t="n"/>
-      <c r="C19" s="108" t="n"/>
-      <c r="D19" s="108" t="n"/>
-      <c r="E19" s="108" t="n"/>
-      <c r="F19" s="108" t="n"/>
-      <c r="G19" s="108" t="n"/>
-      <c r="H19" s="108" t="n"/>
-      <c r="I19" s="109" t="n"/>
+      <c r="A19" s="108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B19" s="108" t="n">
+        <v>900</v>
+      </c>
+      <c r="C19" s="108" t="n">
+        <v>550</v>
+      </c>
+      <c r="D19" s="108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="108" t="inlineStr">
+        <is>
+          <t>banca.blat</t>
+        </is>
+      </c>
+      <c r="F19" s="108" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G19" s="108" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H19" s="108" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I19" s="109" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="J19" s="106" t="n"/>
       <c r="K19" s="110" t="n"/>
       <c r="M19" s="66" t="n"/>

</xml_diff>

<commit_message>
added new dressing architectures
</commit_message>
<xml_diff>
--- a/pythonProject/projects/Comanda Test/Comanda_Proficut_Test.xlsx
+++ b/pythonProject/projects/Comanda Test/Comanda_Proficut_Test.xlsx
@@ -1693,7 +1693,7 @@
         </is>
       </c>
       <c r="B10" s="105" t="n">
-        <v>482</v>
+        <v>1000</v>
       </c>
       <c r="C10" s="105" t="n">
         <v>500</v>
@@ -1703,17 +1703,19 @@
       </c>
       <c r="E10" s="105" t="inlineStr">
         <is>
-          <t>banca.lat1</t>
+          <t>j1.jos</t>
         </is>
       </c>
-      <c r="F10" s="105" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F10" s="105" t="n">
+        <v>1</v>
       </c>
       <c r="G10" s="105" t="inlineStr"/>
-      <c r="H10" s="105" t="inlineStr"/>
-      <c r="I10" s="106" t="inlineStr"/>
+      <c r="H10" s="105" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="106" t="n">
+        <v>1</v>
+      </c>
       <c r="J10" s="106" t="n"/>
       <c r="K10" s="107" t="n"/>
       <c r="W10" s="49">
@@ -1792,7 +1794,7 @@
         </is>
       </c>
       <c r="B11" s="108" t="n">
-        <v>482</v>
+        <v>724</v>
       </c>
       <c r="C11" s="108" t="n">
         <v>500</v>
@@ -1802,13 +1804,11 @@
       </c>
       <c r="E11" s="108" t="inlineStr">
         <is>
-          <t>banca.lat2</t>
+          <t>j1.lat</t>
         </is>
       </c>
-      <c r="F11" s="108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F11" s="108" t="n">
+        <v>1</v>
       </c>
       <c r="G11" s="108" t="inlineStr"/>
       <c r="H11" s="108" t="inlineStr"/>
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="B12" s="108" t="n">
-        <v>764</v>
+        <v>724</v>
       </c>
       <c r="C12" s="108" t="n">
         <v>500</v>
@@ -1902,13 +1902,11 @@
       </c>
       <c r="E12" s="108" t="inlineStr">
         <is>
-          <t>banca.jos</t>
+          <t>j1.lat</t>
         </is>
       </c>
-      <c r="F12" s="108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F12" s="108" t="n">
+        <v>1</v>
       </c>
       <c r="G12" s="108" t="inlineStr"/>
       <c r="H12" s="108" t="inlineStr"/>
@@ -1991,25 +1989,25 @@
         </is>
       </c>
       <c r="B13" s="108" t="n">
-        <v>373</v>
+        <v>962</v>
       </c>
       <c r="C13" s="108" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D13" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="108" t="inlineStr">
         <is>
-          <t>banca.pol1</t>
+          <t>j1.leg1</t>
         </is>
       </c>
-      <c r="F13" s="108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G13" s="108" t="inlineStr"/>
+      <c r="F13" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="108" t="n">
+        <v>1</v>
+      </c>
       <c r="H13" s="108" t="inlineStr"/>
       <c r="I13" s="109" t="inlineStr"/>
       <c r="J13" s="106" t="n"/>
@@ -2091,25 +2089,25 @@
         </is>
       </c>
       <c r="B14" s="108" t="n">
-        <v>382</v>
+        <v>962</v>
       </c>
       <c r="C14" s="108" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D14" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="108" t="inlineStr">
         <is>
-          <t>banca.sep_v</t>
+          <t>j1.leg2</t>
         </is>
       </c>
-      <c r="F14" s="108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G14" s="108" t="inlineStr"/>
+      <c r="F14" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="108" t="n">
+        <v>1</v>
+      </c>
       <c r="H14" s="108" t="inlineStr"/>
       <c r="I14" s="109" t="inlineStr"/>
       <c r="J14" s="106" t="n"/>
@@ -2191,23 +2189,21 @@
         </is>
       </c>
       <c r="B15" s="108" t="n">
-        <v>373</v>
+        <v>964</v>
       </c>
       <c r="C15" s="108" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D15" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="108" t="inlineStr">
         <is>
-          <t>banca.pol2</t>
+          <t>j1.leg</t>
         </is>
       </c>
-      <c r="F15" s="108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F15" s="108" t="n">
+        <v>1</v>
       </c>
       <c r="G15" s="108" t="inlineStr"/>
       <c r="H15" s="108" t="inlineStr"/>
@@ -2291,31 +2287,29 @@
         </is>
       </c>
       <c r="B16" s="108" t="n">
+        <v>600</v>
+      </c>
+      <c r="C16" s="108" t="n">
         <v>500</v>
-      </c>
-      <c r="C16" s="108" t="n">
-        <v>100</v>
       </c>
       <c r="D16" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="108" t="inlineStr">
         <is>
-          <t>banca.plinta1</t>
+          <t>t1.jos</t>
         </is>
       </c>
-      <c r="F16" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G16" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H16" s="108" t="inlineStr"/>
-      <c r="I16" s="109" t="inlineStr"/>
+      <c r="F16" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="108" t="inlineStr"/>
+      <c r="H16" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="109" t="n">
+        <v>1</v>
+      </c>
       <c r="J16" s="106" t="n"/>
       <c r="K16" s="110" t="n"/>
       <c r="M16" s="66" t="n"/>
@@ -2395,30 +2389,26 @@
         </is>
       </c>
       <c r="B17" s="108" t="n">
-        <v>500</v>
+        <v>1952</v>
       </c>
       <c r="C17" s="108" t="n">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="D17" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="108" t="inlineStr">
         <is>
-          <t>banca.plinta2</t>
+          <t>t1.lat</t>
         </is>
       </c>
-      <c r="F17" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G17" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H17" s="108" t="inlineStr"/>
+      <c r="F17" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="108" t="inlineStr"/>
+      <c r="H17" s="108" t="n">
+        <v>1</v>
+      </c>
       <c r="I17" s="109" t="inlineStr"/>
       <c r="J17" s="106" t="n"/>
       <c r="K17" s="110" t="n"/>
@@ -2499,39 +2489,27 @@
         </is>
       </c>
       <c r="B18" s="108" t="n">
-        <v>836</v>
+        <v>1952</v>
       </c>
       <c r="C18" s="108" t="n">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="D18" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="108" t="inlineStr">
         <is>
-          <t>banca.plinta3</t>
+          <t>t1.lat</t>
         </is>
       </c>
-      <c r="F18" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G18" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H18" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I18" s="109" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="F18" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="108" t="inlineStr"/>
+      <c r="H18" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="109" t="inlineStr"/>
       <c r="J18" s="106" t="n"/>
       <c r="K18" s="110" t="n"/>
       <c r="M18" s="66" t="n"/>
@@ -2611,39 +2589,25 @@
         </is>
       </c>
       <c r="B19" s="108" t="n">
-        <v>900</v>
+        <v>564</v>
       </c>
       <c r="C19" s="108" t="n">
-        <v>550</v>
+        <v>499</v>
       </c>
       <c r="D19" s="108" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="108" t="inlineStr">
         <is>
-          <t>banca.blat</t>
+          <t>t1.sus</t>
         </is>
       </c>
-      <c r="F19" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G19" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H19" s="108" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I19" s="109" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="F19" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="108" t="inlineStr"/>
+      <c r="H19" s="108" t="inlineStr"/>
+      <c r="I19" s="109" t="inlineStr"/>
       <c r="J19" s="106" t="n"/>
       <c r="K19" s="110" t="n"/>
       <c r="M19" s="66" t="n"/>
@@ -2717,15 +2681,31 @@
       </c>
     </row>
     <row r="20" ht="18.75" customHeight="1" s="50">
-      <c r="A20" s="108" t="n"/>
-      <c r="B20" s="108" t="n"/>
-      <c r="C20" s="108" t="n"/>
-      <c r="D20" s="108" t="n"/>
-      <c r="E20" s="108" t="n"/>
-      <c r="F20" s="108" t="n"/>
-      <c r="G20" s="108" t="n"/>
-      <c r="H20" s="108" t="n"/>
-      <c r="I20" s="109" t="n"/>
+      <c r="A20" s="108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B20" s="108" t="n">
+        <v>564</v>
+      </c>
+      <c r="C20" s="108" t="n">
+        <v>500</v>
+      </c>
+      <c r="D20" s="108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="108" t="inlineStr">
+        <is>
+          <t>t1.sep.h</t>
+        </is>
+      </c>
+      <c r="F20" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="108" t="inlineStr"/>
+      <c r="H20" s="108" t="inlineStr"/>
+      <c r="I20" s="109" t="inlineStr"/>
       <c r="J20" s="106" t="n"/>
       <c r="K20" s="110" t="n"/>
       <c r="M20" s="48" t="n"/>
@@ -2799,15 +2779,31 @@
       </c>
     </row>
     <row r="21" ht="18.75" customHeight="1" s="50">
-      <c r="A21" s="108" t="n"/>
-      <c r="B21" s="108" t="n"/>
-      <c r="C21" s="108" t="n"/>
-      <c r="D21" s="108" t="n"/>
-      <c r="E21" s="108" t="n"/>
-      <c r="F21" s="108" t="n"/>
-      <c r="G21" s="108" t="n"/>
-      <c r="H21" s="108" t="n"/>
-      <c r="I21" s="109" t="n"/>
+      <c r="A21" s="108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B21" s="108" t="n">
+        <v>564</v>
+      </c>
+      <c r="C21" s="108" t="n">
+        <v>500</v>
+      </c>
+      <c r="D21" s="108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="108" t="inlineStr">
+        <is>
+          <t>t1.sep.h</t>
+        </is>
+      </c>
+      <c r="F21" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="108" t="inlineStr"/>
+      <c r="H21" s="108" t="inlineStr"/>
+      <c r="I21" s="109" t="inlineStr"/>
       <c r="J21" s="109" t="n"/>
       <c r="K21" s="110" t="n"/>
       <c r="M21" s="48" t="n"/>
@@ -2881,15 +2877,31 @@
       </c>
     </row>
     <row r="22" ht="18.75" customHeight="1" s="50">
-      <c r="A22" s="108" t="n"/>
-      <c r="B22" s="108" t="n"/>
-      <c r="C22" s="108" t="n"/>
-      <c r="D22" s="108" t="n"/>
-      <c r="E22" s="108" t="n"/>
-      <c r="F22" s="108" t="n"/>
-      <c r="G22" s="108" t="n"/>
-      <c r="H22" s="108" t="n"/>
-      <c r="I22" s="109" t="n"/>
+      <c r="A22" s="108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B22" s="108" t="n">
+        <v>564</v>
+      </c>
+      <c r="C22" s="108" t="n">
+        <v>500</v>
+      </c>
+      <c r="D22" s="108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="108" t="inlineStr">
+        <is>
+          <t>t1.sep.h</t>
+        </is>
+      </c>
+      <c r="F22" s="108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="108" t="inlineStr"/>
+      <c r="H22" s="108" t="inlineStr"/>
+      <c r="I22" s="109" t="inlineStr"/>
       <c r="J22" s="109" t="n"/>
       <c r="K22" s="110" t="n"/>
       <c r="M22" s="48" t="n"/>

</xml_diff>